<commit_message>
Tweak respiratory volume handling. Lots of documentation updates in preperation for release.
</commit_message>
<xml_diff>
--- a/docs/Figures/PatientWorking.xlsx
+++ b/docs/Figures/PatientWorking.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22228"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D94A455A-CA7B-45BA-A7A2-6A00ABC58914}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7710"/>
+    <workbookView xWindow="14880" yWindow="4470" windowWidth="26595" windowHeight="23535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="22" r:id="rId1"/>
@@ -15,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="906" uniqueCount="177">
   <si>
     <t>Nathan</t>
   </si>
@@ -434,15 +435,6 @@
     <t>\f[Ssa[{m^2}] = 0.20247W{[kg]^{0.45}}H{[m]^{0.725}}\f]</t>
   </si>
   <si>
-    <t>\f[Frc[mL] = 30W[kg]\f]</t>
-  </si>
-  <si>
-    <t>\f[Tlc[mL] = 80W[kg]\f]</t>
-  </si>
-  <si>
-    <t>\f[Rv[mL] = 16W[kg]\f]</t>
-  </si>
-  <si>
     <t>\f[Lbm = W(1 - Ff)\f]</t>
   </si>
   <si>
@@ -452,9 +444,6 @@
     <t>\f[Map = \frac{1}{3}Sys + \frac{2}{3}Dia\f]</t>
   </si>
   <si>
-    <t>\f[Tv[mL] = 37W[kg] - Frc[mL]\f]</t>
-  </si>
-  <si>
     <t>\f[Erv = Frc - Rv\f]</t>
   </si>
   <si>
@@ -537,12 +526,33 @@
   </si>
   <si>
     <t>M = 0.02, F = 0.10</t>
+  </si>
+  <si>
+    <t>Ideal Weight</t>
+  </si>
+  <si>
+    <t>@cite green2017green</t>
+  </si>
+  <si>
+    <t>\f[Frc[mL] = 30Iw[kg]\f]</t>
+  </si>
+  <si>
+    <t>\f[Tlc[mL] = 80Iw[kg]\f]</t>
+  </si>
+  <si>
+    <t>\f[Rv[mL] = 16Iw[kg]\f]</t>
+  </si>
+  <si>
+    <t>\f[Tv[mL] = 37Iw[kg] - Frc[mL]\f]</t>
+  </si>
+  <si>
+    <t>\f[Iw[kg] = \left\{ {\begin{array}{*{20}{c}} {{\rm{50}}{\rm{.0  +  2}}{\rm{.3}}\left( {{\rm{H[in]  -  60}}} \right),\;M}\\ {{\rm{45}}{\rm{.5  +  2}}{\rm{.3}}\left( {{\rm{H[in]  -  60}}} \right),\;F} \end{array}} \right.\f]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -604,6 +614,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -651,7 +664,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -684,9 +697,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -719,6 +749,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -894,11 +941,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -908,7 +955,7 @@
     <col min="3" max="3" width="2.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="2.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="75.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="74.5703125" style="4" customWidth="1"/>
     <col min="7" max="7" width="2.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="2.140625" style="4" bestFit="1" customWidth="1"/>
@@ -930,7 +977,7 @@
         <v>74</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>74</v>
@@ -1018,7 +1065,7 @@
         <v>74</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>74</v>
@@ -1053,7 +1100,7 @@
         <v>74</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>74</v>
@@ -1083,42 +1130,42 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>74</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>29</v>
+        <v>170</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>74</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>74</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>128</v>
+        <v>176</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>74</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>152</v>
+        <v>102</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>74</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>153</v>
+        <v>102</v>
       </c>
       <c r="K5" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="L5" s="4" t="s">
-        <v>154</v>
+      <c r="L5" s="3" t="s">
+        <v>171</v>
       </c>
       <c r="M5" s="4" t="s">
         <v>74</v>
@@ -1129,37 +1176,37 @@
         <v>74</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>74</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>74</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>74</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>105</v>
+        <v>148</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>74</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>172</v>
+        <v>149</v>
       </c>
       <c r="K6" s="4" t="s">
         <v>74</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="M6" s="4" t="s">
         <v>74</v>
@@ -1170,201 +1217,201 @@
         <v>74</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="D7" s="4" t="s">
+      <c r="C8" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="J8" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="M7" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B8" s="4" t="s">
+      <c r="K8" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="F8" s="4" t="s">
+      <c r="C9" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="G8" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="H8" s="4" t="s">
+      <c r="G9" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="H9" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="I8" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="J8" s="4" t="s">
+      <c r="I9" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="J9" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="K8" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="M8" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B9" s="4" t="s">
+      <c r="K9" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="F9" s="4" t="s">
+      <c r="C10" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="G9" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="H9" s="4" t="s">
+      <c r="G10" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="H10" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="I9" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="J9" s="4" t="s">
+      <c r="I10" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="J10" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="K9" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="L9" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="M9" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B10" s="4" t="s">
+      <c r="K10" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="H10" s="4" t="s">
+      <c r="C11" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="H11" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="I10" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="J10" s="4" t="s">
+      <c r="I11" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="J11" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="K10" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="M10" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>50</v>
-      </c>
       <c r="K11" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="L11" s="4" t="s">
-        <v>115</v>
+      <c r="L11" s="3" t="s">
+        <v>162</v>
       </c>
       <c r="M11" s="4" t="s">
         <v>74</v>
@@ -1375,37 +1422,37 @@
         <v>74</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>74</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>74</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>74</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>74</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="K12" s="4" t="s">
         <v>74</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M12" s="4" t="s">
         <v>74</v>
@@ -1416,37 +1463,37 @@
         <v>74</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>74</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>74</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>74</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I13" s="4" t="s">
         <v>74</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="K13" s="4" t="s">
         <v>74</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="M13" s="4" t="s">
         <v>74</v>
@@ -1457,113 +1504,116 @@
         <v>74</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="F14" s="4" t="s">
+      <c r="C15" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F15" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="G14" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="H14" s="4" t="s">
+      <c r="G15" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="H15" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="I14" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="J14" s="4" t="s">
+      <c r="I15" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="J15" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="K14" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="M14" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B15" s="4" t="s">
+      <c r="K15" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="M15" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="F15" s="4" t="s">
+      <c r="C16" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="G15" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="H15" s="4" t="s">
+      <c r="E16" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="H16" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="I15" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="J15" s="4" t="s">
+      <c r="I16" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="J16" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="K15" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="L15" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="M15" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="H16" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="J16" s="4">
-        <v>0.6</v>
-      </c>
       <c r="K16" s="4" t="s">
         <v>74</v>
+      </c>
+      <c r="L16" s="4" t="s">
+        <v>164</v>
       </c>
       <c r="M16" s="4" t="s">
         <v>74</v>
@@ -1574,37 +1624,34 @@
         <v>74</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>74</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>74</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="H17" s="4" t="s">
-        <v>102</v>
+      <c r="H17" s="4">
+        <v>0.5</v>
       </c>
       <c r="I17" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="J17" s="4" t="s">
-        <v>102</v>
+      <c r="J17" s="4">
+        <v>0.6</v>
       </c>
       <c r="K17" s="4" t="s">
         <v>74</v>
-      </c>
-      <c r="L17" s="3" t="s">
-        <v>159</v>
       </c>
       <c r="M17" s="4" t="s">
         <v>74</v>
@@ -1615,19 +1662,19 @@
         <v>74</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>74</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>74</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>163</v>
+        <v>138</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>74</v>
@@ -1645,7 +1692,7 @@
         <v>74</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="M18" s="4" t="s">
         <v>74</v>
@@ -1656,19 +1703,19 @@
         <v>74</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>74</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>74</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>74</v>
@@ -1685,6 +1732,9 @@
       <c r="K19" s="4" t="s">
         <v>74</v>
       </c>
+      <c r="L19" s="3" t="s">
+        <v>156</v>
+      </c>
       <c r="M19" s="4" t="s">
         <v>74</v>
       </c>
@@ -1694,19 +1744,19 @@
         <v>74</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>74</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>74</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>139</v>
+        <v>160</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>74</v>
@@ -1723,9 +1773,6 @@
       <c r="K20" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="L20" s="3" t="s">
-        <v>167</v>
-      </c>
       <c r="M20" s="4" t="s">
         <v>74</v>
       </c>
@@ -1735,19 +1782,19 @@
         <v>74</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>74</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>74</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>140</v>
+        <v>172</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>74</v>
@@ -1765,7 +1812,7 @@
         <v>74</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="M21" s="4" t="s">
         <v>74</v>
@@ -1776,19 +1823,19 @@
         <v>74</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>74</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>74</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>141</v>
+        <v>173</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>74</v>
@@ -1806,7 +1853,7 @@
         <v>74</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="M22" s="4" t="s">
         <v>74</v>
@@ -1817,19 +1864,19 @@
         <v>74</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>74</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>74</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>142</v>
+        <v>174</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>74</v>
@@ -1846,28 +1893,31 @@
       <c r="K23" s="4" t="s">
         <v>74</v>
       </c>
+      <c r="L23" s="3" t="s">
+        <v>163</v>
+      </c>
       <c r="M23" s="4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>74</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>74</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>74</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>74</v>
@@ -1884,31 +1934,28 @@
       <c r="K24" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="L24" s="4" t="s">
-        <v>161</v>
-      </c>
       <c r="M24" s="4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>74</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>74</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>74</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>74</v>
@@ -1925,8 +1972,8 @@
       <c r="K25" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="L25" s="3" t="s">
-        <v>162</v>
+      <c r="L25" s="4" t="s">
+        <v>157</v>
       </c>
       <c r="M25" s="4" t="s">
         <v>74</v>
@@ -1937,19 +1984,19 @@
         <v>74</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>74</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>74</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="G26" s="4" t="s">
         <v>74</v>
@@ -1967,7 +2014,7 @@
         <v>74</v>
       </c>
       <c r="L26" s="3" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="M26" s="4" t="s">
         <v>74</v>
@@ -1978,19 +2025,19 @@
         <v>74</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>74</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>74</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>146</v>
+        <v>175</v>
       </c>
       <c r="G27" s="4" t="s">
         <v>74</v>
@@ -2008,7 +2055,7 @@
         <v>74</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="M27" s="4" t="s">
         <v>74</v>
@@ -2019,19 +2066,19 @@
         <v>74</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>74</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>74</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="G28" s="4" t="s">
         <v>74</v>
@@ -2049,7 +2096,7 @@
         <v>74</v>
       </c>
       <c r="L28" s="3" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="M28" s="4" t="s">
         <v>74</v>
@@ -2060,19 +2107,19 @@
         <v>74</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>74</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>74</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="G29" s="4" t="s">
         <v>74</v>
@@ -2090,7 +2137,7 @@
         <v>74</v>
       </c>
       <c r="L29" s="3" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="M29" s="4" t="s">
         <v>74</v>
@@ -2101,19 +2148,19 @@
         <v>74</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>74</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>74</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="G30" s="4" t="s">
         <v>74</v>
@@ -2131,9 +2178,50 @@
         <v>74</v>
       </c>
       <c r="L30" s="3" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="M30" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="J31" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="K31" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="L31" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="M31" s="4" t="s">
         <v>74</v>
       </c>
     </row>
@@ -2144,7 +2232,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AP24"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Added validation for new respiratory system data. Updated patient methodology table with old change from 16 to 12 bpm. Added outputs to mechanical ventilator scenarios.
</commit_message>
<xml_diff>
--- a/docs/Figures/PatientWorking.xlsx
+++ b/docs/Figures/PatientWorking.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D94A455A-CA7B-45BA-A7A2-6A00ABC58914}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FD02CD8-3400-4FB9-870B-FF9F243DD9F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14880" yWindow="4470" windowWidth="26595" windowHeight="23535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31500" yWindow="5670" windowWidth="23910" windowHeight="22095" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="22" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="906" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="906" uniqueCount="178">
   <si>
     <t>Nathan</t>
   </si>
@@ -426,9 +426,6 @@
     <t>\f[Dia[mmHg] = 73.5\f]</t>
   </si>
   <si>
-    <t>\f[Rr[bpm] = 16\f]</t>
-  </si>
-  <si>
     <t>\f[Rlr = 0.525\f]</t>
   </si>
   <si>
@@ -547,6 +544,12 @@
   </si>
   <si>
     <t>\f[Iw[kg] = \left\{ {\begin{array}{*{20}{c}} {{\rm{50}}{\rm{.0  +  2}}{\rm{.3}}\left( {{\rm{H[in]  -  60}}} \right),\;M}\\ {{\rm{45}}{\rm{.5  +  2}}{\rm{.3}}\left( {{\rm{H[in]  -  60}}} \right),\;F} \end{array}} \right.\f]</t>
+  </si>
+  <si>
+    <t>8 bpm</t>
+  </si>
+  <si>
+    <t>\f[Rr[bpm] = 12\f]</t>
   </si>
 </sst>
 </file>
@@ -945,7 +948,7 @@
   <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -977,7 +980,7 @@
         <v>74</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>74</v>
@@ -1065,7 +1068,7 @@
         <v>74</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>74</v>
@@ -1100,7 +1103,7 @@
         <v>74</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>74</v>
@@ -1135,19 +1138,19 @@
         <v>74</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>74</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>74</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>74</v>
@@ -1165,7 +1168,7 @@
         <v>74</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M5" s="4" t="s">
         <v>74</v>
@@ -1182,7 +1185,7 @@
         <v>74</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>74</v>
@@ -1194,19 +1197,19 @@
         <v>74</v>
       </c>
       <c r="H6" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="J6" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="I6" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="J6" s="4" t="s">
+      <c r="K6" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="L6" s="4" t="s">
         <v>149</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>150</v>
       </c>
       <c r="M6" s="4" t="s">
         <v>74</v>
@@ -1223,7 +1226,7 @@
         <v>74</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>74</v>
@@ -1241,13 +1244,13 @@
         <v>74</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K7" s="4" t="s">
         <v>74</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="M7" s="4" t="s">
         <v>74</v>
@@ -1264,7 +1267,7 @@
         <v>74</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>74</v>
@@ -1282,13 +1285,13 @@
         <v>74</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K8" s="4" t="s">
         <v>74</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M8" s="4" t="s">
         <v>74</v>
@@ -1305,7 +1308,7 @@
         <v>74</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>74</v>
@@ -1329,7 +1332,7 @@
         <v>74</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="M9" s="4" t="s">
         <v>74</v>
@@ -1346,7 +1349,7 @@
         <v>74</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>74</v>
@@ -1370,7 +1373,7 @@
         <v>74</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="M10" s="4" t="s">
         <v>74</v>
@@ -1387,13 +1390,13 @@
         <v>74</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>74</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>74</v>
@@ -1411,7 +1414,7 @@
         <v>74</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="M11" s="4" t="s">
         <v>74</v>
@@ -1428,7 +1431,7 @@
         <v>74</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>74</v>
@@ -1469,7 +1472,7 @@
         <v>74</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>74</v>
@@ -1510,7 +1513,7 @@
         <v>74</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>74</v>
@@ -1551,19 +1554,19 @@
         <v>74</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>74</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>136</v>
+        <v>177</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>74</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>64</v>
+        <v>176</v>
       </c>
       <c r="I15" s="4" t="s">
         <v>74</v>
@@ -1589,13 +1592,13 @@
         <v>74</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>74</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>74</v>
@@ -1613,7 +1616,7 @@
         <v>74</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M16" s="4" t="s">
         <v>74</v>
@@ -1630,13 +1633,13 @@
         <v>74</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>74</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>74</v>
@@ -1668,13 +1671,13 @@
         <v>74</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>74</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>74</v>
@@ -1692,7 +1695,7 @@
         <v>74</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M18" s="4" t="s">
         <v>74</v>
@@ -1709,13 +1712,13 @@
         <v>74</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>74</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>74</v>
@@ -1733,7 +1736,7 @@
         <v>74</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M19" s="4" t="s">
         <v>74</v>
@@ -1750,13 +1753,13 @@
         <v>74</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>74</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>74</v>
@@ -1788,13 +1791,13 @@
         <v>74</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>74</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>74</v>
@@ -1812,7 +1815,7 @@
         <v>74</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="M21" s="4" t="s">
         <v>74</v>
@@ -1829,13 +1832,13 @@
         <v>74</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>74</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>74</v>
@@ -1853,7 +1856,7 @@
         <v>74</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="M22" s="4" t="s">
         <v>74</v>
@@ -1870,13 +1873,13 @@
         <v>74</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>74</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>74</v>
@@ -1894,7 +1897,7 @@
         <v>74</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="M23" s="4" t="s">
         <v>74</v>
@@ -1911,13 +1914,13 @@
         <v>74</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>74</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>74</v>
@@ -1949,13 +1952,13 @@
         <v>74</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>74</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>74</v>
@@ -1973,7 +1976,7 @@
         <v>74</v>
       </c>
       <c r="L25" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="M25" s="4" t="s">
         <v>74</v>
@@ -1990,13 +1993,13 @@
         <v>74</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>74</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G26" s="4" t="s">
         <v>74</v>
@@ -2014,7 +2017,7 @@
         <v>74</v>
       </c>
       <c r="L26" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="M26" s="4" t="s">
         <v>74</v>
@@ -2031,13 +2034,13 @@
         <v>74</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>74</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G27" s="4" t="s">
         <v>74</v>
@@ -2055,7 +2058,7 @@
         <v>74</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="M27" s="4" t="s">
         <v>74</v>
@@ -2072,13 +2075,13 @@
         <v>74</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>74</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G28" s="4" t="s">
         <v>74</v>
@@ -2096,7 +2099,7 @@
         <v>74</v>
       </c>
       <c r="L28" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="M28" s="4" t="s">
         <v>74</v>
@@ -2113,13 +2116,13 @@
         <v>74</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>74</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G29" s="4" t="s">
         <v>74</v>
@@ -2137,7 +2140,7 @@
         <v>74</v>
       </c>
       <c r="L29" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="M29" s="4" t="s">
         <v>74</v>
@@ -2154,13 +2157,13 @@
         <v>74</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>74</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G30" s="4" t="s">
         <v>74</v>
@@ -2178,7 +2181,7 @@
         <v>74</v>
       </c>
       <c r="L30" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="M30" s="4" t="s">
         <v>74</v>
@@ -2195,13 +2198,13 @@
         <v>74</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>74</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G31" s="4" t="s">
         <v>74</v>
@@ -2219,7 +2222,7 @@
         <v>74</v>
       </c>
       <c r="L31" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="M31" s="4" t="s">
         <v>74</v>
@@ -2236,7 +2239,7 @@
   <dimension ref="A1:AP24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+      <selection activeCell="W12" sqref="A1:W12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3016,13 +3019,13 @@
         <v>74</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>74</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>74</v>
@@ -3040,13 +3043,13 @@
         <v>74</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="M11" s="1" t="s">
         <v>74</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>74</v>
@@ -3058,13 +3061,13 @@
         <v>74</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>64</v>
+        <v>176</v>
       </c>
       <c r="S11" s="1" t="s">
         <v>74</v>
       </c>
       <c r="T11" s="1" t="s">
-        <v>64</v>
+        <v>176</v>
       </c>
       <c r="U11" s="1" t="s">
         <v>74</v>

</xml_diff>

<commit_message>
Updates to patient parameters table.
</commit_message>
<xml_diff>
--- a/docs/Figures/PatientWorking.xlsx
+++ b/docs/Figures/PatientWorking.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7DA3761-3B2A-460A-9FB9-2F5833B9F352}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{493CC3B4-D971-423A-B6DC-74DC3CB0F6FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26535" yWindow="6240" windowWidth="28770" windowHeight="21420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2160" yWindow="9765" windowWidth="25275" windowHeight="17355" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="22" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="180">
   <si>
     <t>Nathan</t>
   </si>
@@ -453,15 +453,6 @@
     <t>\f[M = Male,F = Female\f]</t>
   </si>
   <si>
-    <t>Bmi = 16 kg/m&lt;sup&gt;2&lt;/sup&gt;</t>
-  </si>
-  <si>
-    <t>Bmi = 30 kg/m&lt;sup&gt;2&lt;/sup&gt;</t>
-  </si>
-  <si>
-    <t>Bmi = Body Mass Index = W[kg]/H[m]&lt;sup&gt;2&lt;/sup&gt;. 21.75 kg/m&lt;sup&gt;2&lt;/sup&gt; is standard. No severly Underweight or Obese. @cite World2006bmi</t>
-  </si>
-  <si>
     <t>Min = 3rd percentile, Max = 97th percentile, Standard = 50th percentile. @cite Centers2016clinical</t>
   </si>
   <si>
@@ -541,6 +532,30 @@
   </si>
   <si>
     <t>\f[Rr[bpm] = 12\f]</t>
+  </si>
+  <si>
+    <t>Body Mass Index</t>
+  </si>
+  <si>
+    <t>\f[BMI[{\rm{kg/}}{m^2}] = W[kg]/{\rm{H[m}}{{\rm{]}}^2}\f]</t>
+  </si>
+  <si>
+    <t>16 kg/m&lt;sup&gt;2&lt;/sup&gt;</t>
+  </si>
+  <si>
+    <t>30 kg/m&lt;sup&gt;2&lt;/sup&gt;</t>
+  </si>
+  <si>
+    <t>No severly Underweight or Obese. @cite World2006bmi</t>
+  </si>
+  <si>
+    <t>Pulse Pressure Pressure Baseline</t>
+  </si>
+  <si>
+    <t>\f[Pp[mmHg] = Sys[mmHg] - Dia[mmHg]\f]</t>
+  </si>
+  <si>
+    <t>0.25 * Sys</t>
   </si>
 </sst>
 </file>
@@ -936,10 +951,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M30"/>
+  <dimension ref="A1:M32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:M30"/>
+      <selection activeCell="M32" sqref="A1:M32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -953,7 +968,7 @@
     <col min="7" max="7" width="2.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="2.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23" style="4" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="2.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="92.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="2.140625" style="4" bestFit="1" customWidth="1"/>
@@ -971,7 +986,7 @@
         <v>74</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>74</v>
@@ -1094,7 +1109,7 @@
         <v>74</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>74</v>
@@ -1129,19 +1144,19 @@
         <v>74</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>74</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>74</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>74</v>
@@ -1159,13 +1174,13 @@
         <v>74</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="M5" s="4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>74</v>
       </c>
@@ -1176,7 +1191,7 @@
         <v>74</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>74</v>
@@ -1188,19 +1203,16 @@
         <v>74</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>145</v>
+        <v>101</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>74</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>146</v>
+        <v>101</v>
       </c>
       <c r="K6" s="4" t="s">
         <v>74</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>147</v>
       </c>
       <c r="M6" s="4" t="s">
         <v>74</v>
@@ -1217,7 +1229,7 @@
         <v>74</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>74</v>
@@ -1235,177 +1247,177 @@
         <v>74</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="K7" s="4" t="s">
         <v>74</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="M7" s="4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>74</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="F8" s="4" t="s">
+      <c r="C9" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="G8" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="J8" s="4" t="s">
+      <c r="G9" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="J9" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="K8" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="L8" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="M8" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B9" s="4" t="s">
+      <c r="K9" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="F9" s="4" t="s">
+      <c r="C10" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="G9" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="H9" s="4" t="s">
+      <c r="G10" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="H10" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="I9" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="J9" s="4" t="s">
+      <c r="I10" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="J10" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="K9" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="L9" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="M9" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B10" s="4" t="s">
+      <c r="K10" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="F10" s="4" t="s">
+      <c r="C11" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F11" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="G10" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="H10" s="4" t="s">
+      <c r="G11" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="H11" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="I10" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="J10" s="4" t="s">
+      <c r="I11" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="J11" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="K10" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="M10" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>50</v>
-      </c>
       <c r="K11" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="L11" s="4" t="s">
-        <v>114</v>
+      <c r="L11" s="3" t="s">
+        <v>155</v>
       </c>
       <c r="M11" s="4" t="s">
         <v>74</v>
@@ -1416,37 +1428,37 @@
         <v>74</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>74</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>74</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>74</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>74</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="K12" s="4" t="s">
         <v>74</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M12" s="4" t="s">
         <v>74</v>
@@ -1457,37 +1469,37 @@
         <v>74</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>74</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>74</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>74</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I13" s="4" t="s">
         <v>74</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="K13" s="4" t="s">
         <v>74</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M13" s="4" t="s">
         <v>74</v>
@@ -1498,63 +1510,66 @@
         <v>74</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>74</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>74</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>174</v>
+        <v>133</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>74</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>173</v>
+        <v>60</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>74</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K14" s="4" t="s">
         <v>74</v>
       </c>
+      <c r="L14" s="4" t="s">
+        <v>116</v>
+      </c>
       <c r="M14" s="4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>74</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>93</v>
+        <v>177</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>74</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>74</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>157</v>
+        <v>178</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>74</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>101</v>
+        <v>179</v>
       </c>
       <c r="I15" s="4" t="s">
         <v>74</v>
@@ -1565,9 +1580,6 @@
       <c r="K15" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="L15" s="4" t="s">
-        <v>160</v>
-      </c>
       <c r="M15" s="4" t="s">
         <v>74</v>
       </c>
@@ -1577,34 +1589,37 @@
         <v>74</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>74</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>74</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="H16" s="4">
-        <v>0.5</v>
+      <c r="H16" s="4" t="s">
+        <v>101</v>
       </c>
       <c r="I16" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="J16" s="4">
-        <v>0.6</v>
+      <c r="J16" s="4" t="s">
+        <v>101</v>
       </c>
       <c r="K16" s="4" t="s">
         <v>74</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>151</v>
       </c>
       <c r="M16" s="4" t="s">
         <v>74</v>
@@ -1615,60 +1630,57 @@
         <v>74</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>74</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>74</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>135</v>
+        <v>171</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>74</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>101</v>
+        <v>170</v>
       </c>
       <c r="I17" s="4" t="s">
         <v>74</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>101</v>
+        <v>63</v>
       </c>
       <c r="K17" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="L17" s="3" t="s">
-        <v>151</v>
-      </c>
       <c r="M17" s="4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>74</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>74</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>74</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>74</v>
@@ -1685,8 +1697,8 @@
       <c r="K18" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="L18" s="3" t="s">
-        <v>152</v>
+      <c r="L18" s="4" t="s">
+        <v>157</v>
       </c>
       <c r="M18" s="4" t="s">
         <v>74</v>
@@ -1697,31 +1709,31 @@
         <v>74</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>74</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>74</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>156</v>
+        <v>134</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="H19" s="4" t="s">
-        <v>101</v>
+      <c r="H19" s="4">
+        <v>0.5</v>
       </c>
       <c r="I19" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="J19" s="4" t="s">
-        <v>101</v>
+      <c r="J19" s="4">
+        <v>0.6</v>
       </c>
       <c r="K19" s="4" t="s">
         <v>74</v>
@@ -1735,19 +1747,19 @@
         <v>74</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>74</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>74</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>168</v>
+        <v>135</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>74</v>
@@ -1765,7 +1777,7 @@
         <v>74</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="M20" s="4" t="s">
         <v>74</v>
@@ -1776,19 +1788,19 @@
         <v>74</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>74</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>74</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>169</v>
+        <v>152</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>74</v>
@@ -1806,7 +1818,7 @@
         <v>74</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="M21" s="4" t="s">
         <v>74</v>
@@ -1817,19 +1829,19 @@
         <v>74</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>74</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>74</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>74</v>
@@ -1846,9 +1858,6 @@
       <c r="K22" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="L22" s="3" t="s">
-        <v>159</v>
-      </c>
       <c r="M22" s="4" t="s">
         <v>74</v>
       </c>
@@ -1858,19 +1867,19 @@
         <v>74</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>74</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>74</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>136</v>
+        <v>165</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>74</v>
@@ -1887,28 +1896,31 @@
       <c r="K23" s="4" t="s">
         <v>74</v>
       </c>
+      <c r="L23" s="3" t="s">
+        <v>156</v>
+      </c>
       <c r="M23" s="4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>74</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>74</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>74</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>137</v>
+        <v>166</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>74</v>
@@ -1925,8 +1937,8 @@
       <c r="K24" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="L24" s="4" t="s">
-        <v>153</v>
+      <c r="L24" s="3" t="s">
+        <v>156</v>
       </c>
       <c r="M24" s="4" t="s">
         <v>74</v>
@@ -1937,19 +1949,19 @@
         <v>74</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>74</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>74</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>138</v>
+        <v>167</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>74</v>
@@ -1967,7 +1979,7 @@
         <v>74</v>
       </c>
       <c r="L25" s="3" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="M25" s="4" t="s">
         <v>74</v>
@@ -1978,19 +1990,19 @@
         <v>74</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>74</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>74</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>171</v>
+        <v>136</v>
       </c>
       <c r="G26" s="4" t="s">
         <v>74</v>
@@ -2007,31 +2019,28 @@
       <c r="K26" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="L26" s="3" t="s">
+      <c r="M26" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D27" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="M26" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>162</v>
-      </c>
       <c r="E27" s="4" t="s">
         <v>74</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G27" s="4" t="s">
         <v>74</v>
@@ -2048,8 +2057,8 @@
       <c r="K27" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="L27" s="3" t="s">
-        <v>159</v>
+      <c r="L27" s="4" t="s">
+        <v>150</v>
       </c>
       <c r="M27" s="4" t="s">
         <v>74</v>
@@ -2060,19 +2069,19 @@
         <v>74</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>74</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>74</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>140</v>
+        <v>168</v>
       </c>
       <c r="G28" s="4" t="s">
         <v>74</v>
@@ -2090,7 +2099,7 @@
         <v>74</v>
       </c>
       <c r="L28" s="3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="M28" s="4" t="s">
         <v>74</v>
@@ -2101,19 +2110,19 @@
         <v>74</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>74</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>74</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G29" s="4" t="s">
         <v>74</v>
@@ -2131,7 +2140,7 @@
         <v>74</v>
       </c>
       <c r="L29" s="3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="M29" s="4" t="s">
         <v>74</v>
@@ -2142,19 +2151,19 @@
         <v>74</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>74</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>74</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G30" s="4" t="s">
         <v>74</v>
@@ -2172,9 +2181,91 @@
         <v>74</v>
       </c>
       <c r="L30" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="M30" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D31" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="M30" s="4" t="s">
+      <c r="E31" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="J31" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="K31" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="L31" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="M31" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="I32" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="J32" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="K32" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="L32" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="M32" s="4" t="s">
         <v>74</v>
       </c>
     </row>
@@ -3011,13 +3102,13 @@
         <v>74</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="S11" s="1" t="s">
         <v>74</v>
       </c>
       <c r="T11" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="U11" s="1" t="s">
         <v>74</v>

</xml_diff>